<commit_message>
Changes to original data
</commit_message>
<xml_diff>
--- a/Starbucks Excel Analysis.xlsx
+++ b/Starbucks Excel Analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kabooboo\Desktop\Data-Gurus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7866F379-D9F7-49D8-8FCF-044FCFCF637C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A2E5D-501F-4CB6-9DF2-804504A7BB0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final Data'!$K$1:$K$248</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2154,10 +2161,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2667,9 +2674,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2684,10 +2688,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -3055,10 +3062,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K248"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -3103,7 +3110,7 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>696</v>
       </c>
     </row>
@@ -10328,7 +10335,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K1:K248"/>
+  <autoFilter ref="K1:K248" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="A2:L345">
     <sortCondition ref="G2:G345"/>
   </sortState>
@@ -10340,7 +10347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10350,40 +10357,40 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.6328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="3.6328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -10391,21 +10398,21 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A3)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>8</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <f>VLOOKUP(D3,'Final Data'!$G:$J,3,FALSE)</f>
         <v>97069</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f>VLOOKUP(D3,'Final Data'!$G:$J,4,FALSE)</f>
         <v>71204</v>
       </c>
@@ -10414,21 +10421,21 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A4)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>6</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>VLOOKUP(D4,'Final Data'!$G:$J,3,FALSE)</f>
         <v>108092</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>VLOOKUP(D4,'Final Data'!$G:$J,4,FALSE)</f>
         <v>55154</v>
       </c>
@@ -10437,21 +10444,21 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A5)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>5</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f>VLOOKUP(D5,'Final Data'!$G:$J,3,FALSE)</f>
         <v>95622</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f>VLOOKUP(D5,'Final Data'!$G:$J,4,FALSE)</f>
         <v>102304</v>
       </c>
@@ -10460,21 +10467,21 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A6)</f>
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f>VLOOKUP(D6,'Final Data'!$G:$J,3,FALSE)</f>
         <v>76578</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f>VLOOKUP(D6,'Final Data'!$G:$J,4,FALSE)</f>
         <v>37058</v>
       </c>
@@ -10483,21 +10490,21 @@
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A7)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f>VLOOKUP(D7,'Final Data'!$G:$J,3,FALSE)</f>
         <v>62739</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f>VLOOKUP(D7,'Final Data'!$G:$J,4,FALSE)</f>
         <v>265932</v>
       </c>
@@ -10506,21 +10513,21 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A8)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <f>VLOOKUP(D8,'Final Data'!$G:$J,3,FALSE)</f>
         <v>105114</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f>VLOOKUP(D8,'Final Data'!$G:$J,4,FALSE)</f>
         <v>26919</v>
       </c>
@@ -10529,21 +10536,21 @@
       <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A9)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>4</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <f>VLOOKUP(D9,'Final Data'!$G:$J,3,FALSE)</f>
         <v>26006</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <f>VLOOKUP(D9,'Final Data'!$G:$J,4,FALSE)</f>
         <v>39075</v>
       </c>
@@ -10552,21 +10559,21 @@
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A10)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>4</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f>VLOOKUP(D10,'Final Data'!$G:$J,3,FALSE)</f>
         <v>99827</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f>VLOOKUP(D10,'Final Data'!$G:$J,4,FALSE)</f>
         <v>35429</v>
       </c>
@@ -10575,20 +10582,20 @@
       <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A11)</f>
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>4</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>109574</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>4081</v>
       </c>
     </row>
@@ -10596,21 +10603,21 @@
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A12)</f>
         <v>1</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>4</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <f>VLOOKUP(D12,'Final Data'!$G:$J,3,FALSE)</f>
         <v>92826</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f>VLOOKUP(D12,'Final Data'!$G:$J,4,FALSE)</f>
         <v>41795</v>
       </c>
@@ -10619,21 +10626,21 @@
       <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A13)</f>
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>4</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f>VLOOKUP(D13,'Final Data'!$G:$J,3,FALSE)</f>
         <v>34826</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f>VLOOKUP(D13,'Final Data'!$G:$J,4,FALSE)</f>
         <v>282803</v>
       </c>
@@ -10642,21 +10649,21 @@
       <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A14)</f>
         <v>1</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>3</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f>VLOOKUP(D14,'Final Data'!$G:$J,3,FALSE)</f>
         <v>122684</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <f>VLOOKUP(D14,'Final Data'!$G:$J,4,FALSE)</f>
         <v>45336</v>
       </c>
@@ -10665,21 +10672,21 @@
       <c r="A15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A15)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>3</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <f>VLOOKUP(D15,'Final Data'!$G:$J,3,FALSE)</f>
         <v>138906</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <f>VLOOKUP(D15,'Final Data'!$G:$J,4,FALSE)</f>
         <v>3844</v>
       </c>
@@ -10688,21 +10695,21 @@
       <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A16)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>3</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <f>VLOOKUP(D16,'Final Data'!$G:$J,3,FALSE)</f>
         <v>127523</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f>VLOOKUP(D16,'Final Data'!$G:$J,4,FALSE)</f>
         <v>54117</v>
       </c>
@@ -10711,21 +10718,21 @@
       <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A17)</f>
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>3</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <f>VLOOKUP(D17,'Final Data'!$G:$J,3,FALSE)</f>
         <v>49274</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <f>VLOOKUP(D17,'Final Data'!$G:$J,4,FALSE)</f>
         <v>14540</v>
       </c>
@@ -10734,21 +10741,21 @@
       <c r="A18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A18)</f>
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <f>VLOOKUP(D18,'Final Data'!$G:$J,3,FALSE)</f>
         <v>89617</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <f>VLOOKUP(D18,'Final Data'!$G:$J,4,FALSE)</f>
         <v>57695</v>
       </c>
@@ -10757,21 +10764,21 @@
       <c r="A19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A19)</f>
         <v>3</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <f>VLOOKUP(D19,'Final Data'!$G:$J,3,FALSE)</f>
         <v>106599</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <f>VLOOKUP(D19,'Final Data'!$G:$J,4,FALSE)</f>
         <v>24758</v>
       </c>
@@ -10780,21 +10787,21 @@
       <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A20)</f>
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <f>VLOOKUP(D20,'Final Data'!$G:$J,3,FALSE)</f>
         <v>76051</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <f>VLOOKUP(D20,'Final Data'!$G:$J,4,FALSE)</f>
         <v>91415</v>
       </c>
@@ -10803,21 +10810,21 @@
       <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A21)</f>
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>3</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <f>VLOOKUP(D21,'Final Data'!$G:$J,3,FALSE)</f>
         <v>79324</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <f>VLOOKUP(D21,'Final Data'!$G:$J,4,FALSE)</f>
         <v>58499</v>
       </c>
@@ -10826,21 +10833,21 @@
       <c r="A22" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A22)</f>
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>3</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <f>VLOOKUP(D22,'Final Data'!$G:$J,3,FALSE)</f>
         <v>83266</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <f>VLOOKUP(D22,'Final Data'!$G:$J,4,FALSE)</f>
         <v>101639</v>
       </c>
@@ -10849,21 +10856,21 @@
       <c r="A23" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A23)</f>
         <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>2</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <f>VLOOKUP(D23,'Final Data'!$G:$J,3,FALSE)</f>
         <v>129237</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <f>VLOOKUP(D23,'Final Data'!$G:$J,4,FALSE)</f>
         <v>14683</v>
       </c>
@@ -10872,21 +10879,21 @@
       <c r="A24" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A24)</f>
         <v>8</v>
       </c>
       <c r="D24" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>2</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <f>VLOOKUP(D24,'Final Data'!$G:$J,3,FALSE)</f>
         <v>74963</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <f>VLOOKUP(D24,'Final Data'!$G:$J,4,FALSE)</f>
         <v>86207</v>
       </c>
@@ -10895,21 +10902,21 @@
       <c r="A25" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A25)</f>
         <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>2</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <f>VLOOKUP(D25,'Final Data'!$G:$J,3,FALSE)</f>
         <v>130670</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <f>VLOOKUP(D25,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8710</v>
       </c>
@@ -10918,21 +10925,21 @@
       <c r="A26" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A26)</f>
         <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>2</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <f>VLOOKUP(D26,'Final Data'!$G:$J,3,FALSE)</f>
         <v>122848</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <f>VLOOKUP(D26,'Final Data'!$G:$J,4,FALSE)</f>
         <v>23972</v>
       </c>
@@ -10941,21 +10948,21 @@
       <c r="A27" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A27)</f>
         <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>149</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>2</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <f>VLOOKUP(D27,'Final Data'!$G:$J,3,FALSE)</f>
         <v>116078</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <f>VLOOKUP(D27,'Final Data'!$G:$J,4,FALSE)</f>
         <v>16822</v>
       </c>
@@ -10964,21 +10971,21 @@
       <c r="A28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A28)</f>
         <v>2</v>
       </c>
       <c r="D28" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>2</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <f>VLOOKUP(D28,'Final Data'!$G:$J,3,FALSE)</f>
         <v>121769</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <f>VLOOKUP(D28,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11241</v>
       </c>
@@ -10987,21 +10994,21 @@
       <c r="A29" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A29)</f>
         <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>169</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>2</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <f>VLOOKUP(D29,'Final Data'!$G:$J,3,FALSE)</f>
         <v>77400</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <f>VLOOKUP(D29,'Final Data'!$G:$J,4,FALSE)</f>
         <v>9433</v>
       </c>
@@ -11010,21 +11017,21 @@
       <c r="A30" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A30)</f>
         <v>3</v>
       </c>
       <c r="D30" t="s">
         <v>174</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>2</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <f>VLOOKUP(D30,'Final Data'!$G:$J,3,FALSE)</f>
         <v>103505</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <f>VLOOKUP(D30,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12165</v>
       </c>
@@ -11033,21 +11040,21 @@
       <c r="A31" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A31)</f>
         <v>2</v>
       </c>
       <c r="D31" t="s">
         <v>258</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>2</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <f>VLOOKUP(D31,'Final Data'!$G:$J,3,FALSE)</f>
         <v>59277</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="7">
         <f>VLOOKUP(D31,'Final Data'!$G:$J,4,FALSE)</f>
         <v>44673</v>
       </c>
@@ -11056,21 +11063,21 @@
       <c r="A32" t="s">
         <v>144</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A32)</f>
         <v>1</v>
       </c>
       <c r="D32" t="s">
         <v>265</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>2</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <f>VLOOKUP(D32,'Final Data'!$G:$J,3,FALSE)</f>
         <v>63940</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <f>VLOOKUP(D32,'Final Data'!$G:$J,4,FALSE)</f>
         <v>9569</v>
       </c>
@@ -11079,21 +11086,21 @@
       <c r="A33" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A33)</f>
         <v>2</v>
       </c>
       <c r="D33" t="s">
         <v>380</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>2</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <f>VLOOKUP(D33,'Final Data'!$G:$J,3,FALSE)</f>
         <v>113293</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="7">
         <f>VLOOKUP(D33,'Final Data'!$G:$J,4,FALSE)</f>
         <v>38572</v>
       </c>
@@ -11102,21 +11109,21 @@
       <c r="A34" t="s">
         <v>155</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A34)</f>
         <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>388</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>2</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <f>VLOOKUP(D34,'Final Data'!$G:$J,3,FALSE)</f>
         <v>133902</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="7">
         <f>VLOOKUP(D34,'Final Data'!$G:$J,4,FALSE)</f>
         <v>20568</v>
       </c>
@@ -11125,21 +11132,21 @@
       <c r="A35" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A35)</f>
         <v>1</v>
       </c>
       <c r="D35" t="s">
         <v>399</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>2</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <f>VLOOKUP(D35,'Final Data'!$G:$J,3,FALSE)</f>
         <v>92296</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <f>VLOOKUP(D35,'Final Data'!$G:$J,4,FALSE)</f>
         <v>18833</v>
       </c>
@@ -11148,21 +11155,21 @@
       <c r="A36" t="s">
         <v>161</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A36)</f>
         <v>2</v>
       </c>
       <c r="D36" t="s">
         <v>416</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>2</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="7">
         <f>VLOOKUP(D36,'Final Data'!$G:$J,3,FALSE)</f>
         <v>38413</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="7">
         <f>VLOOKUP(D36,'Final Data'!$G:$J,4,FALSE)</f>
         <v>56792</v>
       </c>
@@ -11171,21 +11178,21 @@
       <c r="A37" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A37)</f>
         <v>1</v>
       </c>
       <c r="D37" t="s">
         <v>435</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>2</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <f>VLOOKUP(D37,'Final Data'!$G:$J,3,FALSE)</f>
         <v>57269</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="7">
         <f>VLOOKUP(D37,'Final Data'!$G:$J,4,FALSE)</f>
         <v>63438</v>
       </c>
@@ -11194,21 +11201,21 @@
       <c r="A38" t="s">
         <v>169</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A38)</f>
         <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>441</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>2</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="7">
         <f>VLOOKUP(D38,'Final Data'!$G:$J,3,FALSE)</f>
         <v>88723</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="7">
         <f>VLOOKUP(D38,'Final Data'!$G:$J,4,FALSE)</f>
         <v>42591</v>
       </c>
@@ -11217,21 +11224,21 @@
       <c r="A39" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A39)</f>
         <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>508</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
         <v>2</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="8">
         <f>VLOOKUP(D39,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="8">
         <f>VLOOKUP(D39,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11240,21 +11247,21 @@
       <c r="A40" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A40)</f>
         <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>514</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="6">
         <v>2</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="7">
         <f>VLOOKUP(D40,'Final Data'!$G:$J,3,FALSE)</f>
         <v>137768</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="7">
         <f>VLOOKUP(D40,'Final Data'!$G:$J,4,FALSE)</f>
         <v>15121</v>
       </c>
@@ -11263,21 +11270,21 @@
       <c r="A41" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A41)</f>
         <v>5</v>
       </c>
       <c r="D41" t="s">
         <v>522</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="6">
         <v>2</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="7">
         <f>VLOOKUP(D41,'Final Data'!$G:$J,3,FALSE)</f>
         <v>162011</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="7">
         <f>VLOOKUP(D41,'Final Data'!$G:$J,4,FALSE)</f>
         <v>25554</v>
       </c>
@@ -11286,21 +11293,21 @@
       <c r="A42" t="s">
         <v>193</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A42)</f>
         <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>553</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="6">
         <v>2</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="7">
         <f>VLOOKUP(D42,'Final Data'!$G:$J,3,FALSE)</f>
         <v>99883</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="7">
         <f>VLOOKUP(D42,'Final Data'!$G:$J,4,FALSE)</f>
         <v>19279</v>
       </c>
@@ -11309,21 +11316,21 @@
       <c r="A43" t="s">
         <v>194</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A43)</f>
         <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>560</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="6">
         <v>2</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="8">
         <f>VLOOKUP(D43,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="8">
         <f>VLOOKUP(D43,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11332,21 +11339,21 @@
       <c r="A44" t="s">
         <v>199</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A44)</f>
         <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>571</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="6">
         <v>2</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="8">
         <f>VLOOKUP(D44,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="8">
         <f>VLOOKUP(D44,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11355,21 +11362,21 @@
       <c r="A45" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A45)</f>
         <v>1</v>
       </c>
       <c r="D45" t="s">
         <v>586</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>2</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7">
         <f>VLOOKUP(D45,'Final Data'!$G:$J,3,FALSE)</f>
         <v>65074</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="7">
         <f>VLOOKUP(D45,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8811</v>
       </c>
@@ -11378,21 +11385,21 @@
       <c r="A46" t="s">
         <v>205</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A46)</f>
         <v>1</v>
       </c>
       <c r="D46" t="s">
         <v>618</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="6">
         <v>2</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="8">
         <f>VLOOKUP(D46,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="8">
         <f>VLOOKUP(D46,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11401,21 +11408,21 @@
       <c r="A47" t="s">
         <v>208</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A47)</f>
         <v>1</v>
       </c>
       <c r="D47" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="7">
-        <v>1</v>
-      </c>
-      <c r="F47" s="8">
+      <c r="E47" s="6">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7">
         <f>VLOOKUP(D47,'Final Data'!$G:$J,3,FALSE)</f>
         <v>63887</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="7">
         <f>VLOOKUP(D47,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8370</v>
       </c>
@@ -11424,21 +11431,21 @@
       <c r="A48" t="s">
         <v>209</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A48)</f>
         <v>1</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="7">
-        <v>1</v>
-      </c>
-      <c r="F48" s="8">
+      <c r="E48" s="6">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
         <f>VLOOKUP(D48,'Final Data'!$G:$J,3,FALSE)</f>
         <v>151875</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="7">
         <f>VLOOKUP(D48,'Final Data'!$G:$J,4,FALSE)</f>
         <v>6820</v>
       </c>
@@ -11447,21 +11454,21 @@
       <c r="A49" t="s">
         <v>214</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A49)</f>
         <v>1</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="7">
-        <v>1</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E49" s="6">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
         <f>VLOOKUP(D49,'Final Data'!$G:$J,3,FALSE)</f>
         <v>39324</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="7">
         <f>VLOOKUP(D49,'Final Data'!$G:$J,4,FALSE)</f>
         <v>15830</v>
       </c>
@@ -11470,21 +11477,21 @@
       <c r="A50" t="s">
         <v>217</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A50)</f>
         <v>5</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
       </c>
-      <c r="E50" s="7">
-        <v>1</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="E50" s="6">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7">
         <f>VLOOKUP(D50,'Final Data'!$G:$J,3,FALSE)</f>
         <v>69877</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="7">
         <f>VLOOKUP(D50,'Final Data'!$G:$J,4,FALSE)</f>
         <v>22141</v>
       </c>
@@ -11493,21 +11500,21 @@
       <c r="A51" t="s">
         <v>230</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A51)</f>
         <v>1</v>
       </c>
       <c r="D51" t="s">
         <v>35</v>
       </c>
-      <c r="E51" s="7">
-        <v>1</v>
-      </c>
-      <c r="F51" s="9">
+      <c r="E51" s="6">
+        <v>1</v>
+      </c>
+      <c r="F51" s="8">
         <f>VLOOKUP(D51,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="8">
         <f>VLOOKUP(D51,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11516,21 +11523,21 @@
       <c r="A52" t="s">
         <v>231</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A52)</f>
         <v>1</v>
       </c>
       <c r="D52" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="7">
-        <v>1</v>
-      </c>
-      <c r="F52" s="8">
+      <c r="E52" s="6">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7">
         <f>VLOOKUP(D52,'Final Data'!$G:$J,3,FALSE)</f>
         <v>56701</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="7">
         <f>VLOOKUP(D52,'Final Data'!$G:$J,4,FALSE)</f>
         <v>66719</v>
       </c>
@@ -11539,21 +11546,21 @@
       <c r="A53" t="s">
         <v>236</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A53)</f>
         <v>1</v>
       </c>
       <c r="D53" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="7">
-        <v>1</v>
-      </c>
-      <c r="F53" s="8">
+      <c r="E53" s="6">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7">
         <f>VLOOKUP(D53,'Final Data'!$G:$J,3,FALSE)</f>
         <v>104452</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="7">
         <f>VLOOKUP(D53,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8244</v>
       </c>
@@ -11562,21 +11569,21 @@
       <c r="A54" t="s">
         <v>239</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A54)</f>
         <v>4</v>
       </c>
       <c r="D54" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="7">
-        <v>1</v>
-      </c>
-      <c r="F54" s="9">
+      <c r="E54" s="6">
+        <v>1</v>
+      </c>
+      <c r="F54" s="8">
         <f>VLOOKUP(D54,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="8">
         <f>VLOOKUP(D54,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11585,21 +11592,21 @@
       <c r="A55" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A55)</f>
         <v>1</v>
       </c>
       <c r="D55" t="s">
         <v>47</v>
       </c>
-      <c r="E55" s="7">
-        <v>1</v>
-      </c>
-      <c r="F55" s="9">
+      <c r="E55" s="6">
+        <v>1</v>
+      </c>
+      <c r="F55" s="8">
         <f>VLOOKUP(D55,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="8">
         <f>VLOOKUP(D55,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11608,21 +11615,21 @@
       <c r="A56" t="s">
         <v>248</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A56)</f>
         <v>1</v>
       </c>
       <c r="D56" t="s">
         <v>51</v>
       </c>
-      <c r="E56" s="7">
-        <v>1</v>
-      </c>
-      <c r="F56" s="8">
+      <c r="E56" s="6">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7">
         <f>VLOOKUP(D56,'Final Data'!$G:$J,3,FALSE)</f>
         <v>150635</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="7">
         <f>VLOOKUP(D56,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7792</v>
       </c>
@@ -11631,21 +11638,21 @@
       <c r="A57" t="s">
         <v>251</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A57)</f>
         <v>1</v>
       </c>
       <c r="D57" t="s">
         <v>55</v>
       </c>
-      <c r="E57" s="7">
-        <v>1</v>
-      </c>
-      <c r="F57" s="9">
+      <c r="E57" s="6">
+        <v>1</v>
+      </c>
+      <c r="F57" s="8">
         <f>VLOOKUP(D57,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="8">
         <f>VLOOKUP(D57,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11654,21 +11661,21 @@
       <c r="A58" t="s">
         <v>253</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A58)</f>
         <v>1</v>
       </c>
       <c r="D58" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="7">
-        <v>1</v>
-      </c>
-      <c r="F58" s="8">
+      <c r="E58" s="6">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7">
         <f>VLOOKUP(D58,'Final Data'!$G:$J,3,FALSE)</f>
         <v>91055</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="7">
         <f>VLOOKUP(D58,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8390</v>
       </c>
@@ -11677,21 +11684,21 @@
       <c r="A59" t="s">
         <v>257</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A59)</f>
         <v>1</v>
       </c>
       <c r="D59" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="7">
-        <v>1</v>
-      </c>
-      <c r="F59" s="8">
+      <c r="E59" s="6">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7">
         <f>VLOOKUP(D59,'Final Data'!$G:$J,3,FALSE)</f>
         <v>85640</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="7">
         <f>VLOOKUP(D59,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11808</v>
       </c>
@@ -11700,21 +11707,21 @@
       <c r="A60" t="s">
         <v>258</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A60)</f>
         <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>69</v>
       </c>
-      <c r="E60" s="7">
-        <v>1</v>
-      </c>
-      <c r="F60" s="8">
+      <c r="E60" s="6">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7">
         <f>VLOOKUP(D60,'Final Data'!$G:$J,3,FALSE)</f>
         <v>73051</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="7">
         <f>VLOOKUP(D60,'Final Data'!$G:$J,4,FALSE)</f>
         <v>75118</v>
       </c>
@@ -11723,21 +11730,21 @@
       <c r="A61" t="s">
         <v>265</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A61)</f>
         <v>2</v>
       </c>
       <c r="D61" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="7">
-        <v>1</v>
-      </c>
-      <c r="F61" s="8">
+      <c r="E61" s="6">
+        <v>1</v>
+      </c>
+      <c r="F61" s="7">
         <f>VLOOKUP(D61,'Final Data'!$G:$J,3,FALSE)</f>
         <v>50709</v>
       </c>
-      <c r="G61" s="8">
+      <c r="G61" s="7">
         <f>VLOOKUP(D61,'Final Data'!$G:$J,4,FALSE)</f>
         <v>9835</v>
       </c>
@@ -11746,21 +11753,21 @@
       <c r="A62" t="s">
         <v>268</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A62)</f>
         <v>1</v>
       </c>
       <c r="D62" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="7">
-        <v>1</v>
-      </c>
-      <c r="F62" s="8">
+      <c r="E62" s="6">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7">
         <f>VLOOKUP(D62,'Final Data'!$G:$J,3,FALSE)</f>
         <v>26105</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="7">
         <f>VLOOKUP(D62,'Final Data'!$G:$J,4,FALSE)</f>
         <v>75550</v>
       </c>
@@ -11769,21 +11776,21 @@
       <c r="A63" t="s">
         <v>272</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A63)</f>
         <v>1</v>
       </c>
       <c r="D63" t="s">
         <v>86</v>
       </c>
-      <c r="E63" s="7">
-        <v>1</v>
-      </c>
-      <c r="F63" s="9">
+      <c r="E63" s="6">
+        <v>1</v>
+      </c>
+      <c r="F63" s="8">
         <f>VLOOKUP(D63,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="8">
         <f>VLOOKUP(D63,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11792,21 +11799,21 @@
       <c r="A64" t="s">
         <v>275</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A64)</f>
         <v>1</v>
       </c>
       <c r="D64" t="s">
         <v>87</v>
       </c>
-      <c r="E64" s="7">
-        <v>1</v>
-      </c>
-      <c r="F64" s="8">
+      <c r="E64" s="6">
+        <v>1</v>
+      </c>
+      <c r="F64" s="7">
         <f>VLOOKUP(D64,'Final Data'!$G:$J,3,FALSE)</f>
         <v>176364</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="7">
         <f>VLOOKUP(D64,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10507</v>
       </c>
@@ -11815,21 +11822,21 @@
       <c r="A65" t="s">
         <v>276</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A65)</f>
         <v>1</v>
       </c>
       <c r="D65" t="s">
         <v>111</v>
       </c>
-      <c r="E65" s="7">
-        <v>1</v>
-      </c>
-      <c r="F65" s="8">
+      <c r="E65" s="6">
+        <v>1</v>
+      </c>
+      <c r="F65" s="7">
         <f>VLOOKUP(D65,'Final Data'!$G:$J,3,FALSE)</f>
         <v>101375</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G65" s="7">
         <f>VLOOKUP(D65,'Final Data'!$G:$J,4,FALSE)</f>
         <v>1540</v>
       </c>
@@ -11838,21 +11845,21 @@
       <c r="A66" t="s">
         <v>278</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A66)</f>
         <v>1</v>
       </c>
       <c r="D66" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="7">
-        <v>1</v>
-      </c>
-      <c r="F66" s="8">
+      <c r="E66" s="6">
+        <v>1</v>
+      </c>
+      <c r="F66" s="7">
         <f>VLOOKUP(D66,'Final Data'!$G:$J,3,FALSE)</f>
         <v>100192</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G66" s="7">
         <f>VLOOKUP(D66,'Final Data'!$G:$J,4,FALSE)</f>
         <v>15607</v>
       </c>
@@ -11861,21 +11868,21 @@
       <c r="A67" t="s">
         <v>282</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A67)</f>
         <v>1</v>
       </c>
       <c r="D67" t="s">
         <v>119</v>
       </c>
-      <c r="E67" s="7">
-        <v>1</v>
-      </c>
-      <c r="F67" s="8">
+      <c r="E67" s="6">
+        <v>1</v>
+      </c>
+      <c r="F67" s="7">
         <f>VLOOKUP(D67,'Final Data'!$G:$J,3,FALSE)</f>
         <v>52634</v>
       </c>
-      <c r="G67" s="8">
+      <c r="G67" s="7">
         <f>VLOOKUP(D67,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4933</v>
       </c>
@@ -11884,21 +11891,21 @@
       <c r="A68" t="s">
         <v>286</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A68)</f>
         <v>3</v>
       </c>
       <c r="D68" t="s">
         <v>144</v>
       </c>
-      <c r="E68" s="7">
-        <v>1</v>
-      </c>
-      <c r="F68" s="8">
+      <c r="E68" s="6">
+        <v>1</v>
+      </c>
+      <c r="F68" s="7">
         <f>VLOOKUP(D68,'Final Data'!$G:$J,3,FALSE)</f>
         <v>94321</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="7">
         <f>VLOOKUP(D68,'Final Data'!$G:$J,4,FALSE)</f>
         <v>16747</v>
       </c>
@@ -11907,21 +11914,21 @@
       <c r="A69" t="s">
         <v>295</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A69)</f>
         <v>1</v>
       </c>
       <c r="D69" t="s">
         <v>155</v>
       </c>
-      <c r="E69" s="7">
-        <v>1</v>
-      </c>
-      <c r="F69" s="8">
+      <c r="E69" s="6">
+        <v>1</v>
+      </c>
+      <c r="F69" s="7">
         <f>VLOOKUP(D69,'Final Data'!$G:$J,3,FALSE)</f>
         <v>67983</v>
       </c>
-      <c r="G69" s="8">
+      <c r="G69" s="7">
         <f>VLOOKUP(D69,'Final Data'!$G:$J,4,FALSE)</f>
         <v>30556</v>
       </c>
@@ -11930,21 +11937,21 @@
       <c r="A70" t="s">
         <v>298</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A70)</f>
         <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>158</v>
       </c>
-      <c r="E70" s="7">
-        <v>1</v>
-      </c>
-      <c r="F70" s="8">
+      <c r="E70" s="6">
+        <v>1</v>
+      </c>
+      <c r="F70" s="7">
         <f>VLOOKUP(D70,'Final Data'!$G:$J,3,FALSE)</f>
         <v>105959</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="7">
         <f>VLOOKUP(D70,'Final Data'!$G:$J,4,FALSE)</f>
         <v>48673</v>
       </c>
@@ -11953,21 +11960,21 @@
       <c r="A71" t="s">
         <v>300</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A71)</f>
         <v>5</v>
       </c>
       <c r="D71" t="s">
         <v>166</v>
       </c>
-      <c r="E71" s="7">
-        <v>1</v>
-      </c>
-      <c r="F71" s="9">
+      <c r="E71" s="6">
+        <v>1</v>
+      </c>
+      <c r="F71" s="8">
         <f>VLOOKUP(D71,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="8">
         <f>VLOOKUP(D71,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -11976,21 +11983,21 @@
       <c r="A72" t="s">
         <v>314</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A72)</f>
         <v>1</v>
       </c>
       <c r="D72" t="s">
         <v>172</v>
       </c>
-      <c r="E72" s="7">
-        <v>1</v>
-      </c>
-      <c r="F72" s="8">
+      <c r="E72" s="6">
+        <v>1</v>
+      </c>
+      <c r="F72" s="7">
         <f>VLOOKUP(D72,'Final Data'!$G:$J,3,FALSE)</f>
         <v>66470</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="7">
         <f>VLOOKUP(D72,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12258</v>
       </c>
@@ -11999,21 +12006,21 @@
       <c r="A73" t="s">
         <v>318</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A73)</f>
         <v>1</v>
       </c>
       <c r="D73" t="s">
         <v>193</v>
       </c>
-      <c r="E73" s="7">
-        <v>1</v>
-      </c>
-      <c r="F73" s="8">
+      <c r="E73" s="6">
+        <v>1</v>
+      </c>
+      <c r="F73" s="7">
         <f>VLOOKUP(D73,'Final Data'!$G:$J,3,FALSE)</f>
         <v>45186</v>
       </c>
-      <c r="G73" s="8">
+      <c r="G73" s="7">
         <f>VLOOKUP(D73,'Final Data'!$G:$J,4,FALSE)</f>
         <v>129363</v>
       </c>
@@ -12022,21 +12029,21 @@
       <c r="A74" t="s">
         <v>322</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A74)</f>
         <v>4</v>
       </c>
       <c r="D74" t="s">
         <v>194</v>
       </c>
-      <c r="E74" s="7">
-        <v>1</v>
-      </c>
-      <c r="F74" s="8">
+      <c r="E74" s="6">
+        <v>1</v>
+      </c>
+      <c r="F74" s="7">
         <f>VLOOKUP(D74,'Final Data'!$G:$J,3,FALSE)</f>
         <v>80670</v>
       </c>
-      <c r="G74" s="8">
+      <c r="G74" s="7">
         <f>VLOOKUP(D74,'Final Data'!$G:$J,4,FALSE)</f>
         <v>28509</v>
       </c>
@@ -12045,21 +12052,21 @@
       <c r="A75" t="s">
         <v>330</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A75)</f>
         <v>1</v>
       </c>
       <c r="D75" t="s">
         <v>199</v>
       </c>
-      <c r="E75" s="7">
-        <v>1</v>
-      </c>
-      <c r="F75" s="8">
+      <c r="E75" s="6">
+        <v>1</v>
+      </c>
+      <c r="F75" s="7">
         <f>VLOOKUP(D75,'Final Data'!$G:$J,3,FALSE)</f>
         <v>94395</v>
       </c>
-      <c r="G75" s="8">
+      <c r="G75" s="7">
         <f>VLOOKUP(D75,'Final Data'!$G:$J,4,FALSE)</f>
         <v>45489</v>
       </c>
@@ -12068,21 +12075,21 @@
       <c r="A76" t="s">
         <v>331</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A76)</f>
         <v>1</v>
       </c>
       <c r="D76" t="s">
         <v>202</v>
       </c>
-      <c r="E76" s="7">
-        <v>1</v>
-      </c>
-      <c r="F76" s="8">
+      <c r="E76" s="6">
+        <v>1</v>
+      </c>
+      <c r="F76" s="7">
         <f>VLOOKUP(D76,'Final Data'!$G:$J,3,FALSE)</f>
         <v>52602</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76" s="7">
         <f>VLOOKUP(D76,'Final Data'!$G:$J,4,FALSE)</f>
         <v>6300</v>
       </c>
@@ -12091,21 +12098,21 @@
       <c r="A77" t="s">
         <v>336</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A77)</f>
         <v>1</v>
       </c>
       <c r="D77" t="s">
         <v>205</v>
       </c>
-      <c r="E77" s="7">
-        <v>1</v>
-      </c>
-      <c r="F77" s="9">
+      <c r="E77" s="6">
+        <v>1</v>
+      </c>
+      <c r="F77" s="8">
         <f>VLOOKUP(D77,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="8">
         <f>VLOOKUP(D77,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12114,21 +12121,21 @@
       <c r="A78" t="s">
         <v>337</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A78)</f>
         <v>1</v>
       </c>
       <c r="D78" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="7">
-        <v>1</v>
-      </c>
-      <c r="F78" s="8">
+      <c r="E78" s="6">
+        <v>1</v>
+      </c>
+      <c r="F78" s="7">
         <f>VLOOKUP(D78,'Final Data'!$G:$J,3,FALSE)</f>
         <v>60869</v>
       </c>
-      <c r="G78" s="8">
+      <c r="G78" s="7">
         <f>VLOOKUP(D78,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4650</v>
       </c>
@@ -12137,21 +12144,21 @@
       <c r="A79" t="s">
         <v>339</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A79)</f>
         <v>1</v>
       </c>
       <c r="D79" t="s">
         <v>209</v>
       </c>
-      <c r="E79" s="7">
-        <v>1</v>
-      </c>
-      <c r="F79" s="8">
+      <c r="E79" s="6">
+        <v>1</v>
+      </c>
+      <c r="F79" s="7">
         <f>VLOOKUP(D79,'Final Data'!$G:$J,3,FALSE)</f>
         <v>123266</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79" s="7">
         <f>VLOOKUP(D79,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11792</v>
       </c>
@@ -12160,21 +12167,21 @@
       <c r="A80" t="s">
         <v>343</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A80)</f>
         <v>1</v>
       </c>
       <c r="D80" t="s">
         <v>214</v>
       </c>
-      <c r="E80" s="7">
-        <v>1</v>
-      </c>
-      <c r="F80" s="9">
+      <c r="E80" s="6">
+        <v>1</v>
+      </c>
+      <c r="F80" s="8">
         <f>VLOOKUP(D80,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G80" s="9">
+      <c r="G80" s="8">
         <f>VLOOKUP(D80,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12183,21 +12190,21 @@
       <c r="A81" t="s">
         <v>346</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A81)</f>
         <v>1</v>
       </c>
       <c r="D81" t="s">
         <v>230</v>
       </c>
-      <c r="E81" s="7">
-        <v>1</v>
-      </c>
-      <c r="F81" s="8">
+      <c r="E81" s="6">
+        <v>1</v>
+      </c>
+      <c r="F81" s="7">
         <f>VLOOKUP(D81,'Final Data'!$G:$J,3,FALSE)</f>
         <v>57232</v>
       </c>
-      <c r="G81" s="8">
+      <c r="G81" s="7">
         <f>VLOOKUP(D81,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4849</v>
       </c>
@@ -12206,21 +12213,21 @@
       <c r="A82" t="s">
         <v>349</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A82)</f>
         <v>1</v>
       </c>
       <c r="D82" t="s">
         <v>231</v>
       </c>
-      <c r="E82" s="7">
-        <v>1</v>
-      </c>
-      <c r="F82" s="8">
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="7">
         <f>VLOOKUP(D82,'Final Data'!$G:$J,3,FALSE)</f>
         <v>155458</v>
       </c>
-      <c r="G82" s="8">
+      <c r="G82" s="7">
         <f>VLOOKUP(D82,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10953</v>
       </c>
@@ -12229,21 +12236,21 @@
       <c r="A83" t="s">
         <v>352</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A83)</f>
         <v>1</v>
       </c>
       <c r="D83" t="s">
         <v>236</v>
       </c>
-      <c r="E83" s="7">
-        <v>1</v>
-      </c>
-      <c r="F83" s="9">
+      <c r="E83" s="6">
+        <v>1</v>
+      </c>
+      <c r="F83" s="8">
         <f>VLOOKUP(D83,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="8">
         <f>VLOOKUP(D83,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12252,21 +12259,21 @@
       <c r="A84" t="s">
         <v>353</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A84)</f>
         <v>1</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
       </c>
-      <c r="E84" s="7">
-        <v>1</v>
-      </c>
-      <c r="F84" s="8">
+      <c r="E84" s="6">
+        <v>1</v>
+      </c>
+      <c r="F84" s="7">
         <f>VLOOKUP(D84,'Final Data'!$G:$J,3,FALSE)</f>
         <v>65000</v>
       </c>
-      <c r="G84" s="8">
+      <c r="G84" s="7">
         <f>VLOOKUP(D84,'Final Data'!$G:$J,4,FALSE)</f>
         <v>37029</v>
       </c>
@@ -12275,21 +12282,21 @@
       <c r="A85" t="s">
         <v>359</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A85)</f>
         <v>1</v>
       </c>
       <c r="D85" t="s">
         <v>248</v>
       </c>
-      <c r="E85" s="7">
-        <v>1</v>
-      </c>
-      <c r="F85" s="9">
+      <c r="E85" s="6">
+        <v>1</v>
+      </c>
+      <c r="F85" s="8">
         <f>VLOOKUP(D85,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="9">
+      <c r="G85" s="8">
         <f>VLOOKUP(D85,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12298,21 +12305,21 @@
       <c r="A86" t="s">
         <v>360</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A86)</f>
         <v>1</v>
       </c>
       <c r="D86" t="s">
         <v>251</v>
       </c>
-      <c r="E86" s="7">
-        <v>1</v>
-      </c>
-      <c r="F86" s="10">
+      <c r="E86" s="6">
+        <v>1</v>
+      </c>
+      <c r="F86" s="9">
         <f>VLOOKUP(D86,'Final Data'!$G:$J,3,FALSE)</f>
         <v>196821</v>
       </c>
-      <c r="G86" s="10">
+      <c r="G86" s="9">
         <f>VLOOKUP(D86,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7668</v>
       </c>
@@ -12321,21 +12328,21 @@
       <c r="A87" t="s">
         <v>365</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A87)</f>
         <v>1</v>
       </c>
       <c r="D87" t="s">
         <v>253</v>
       </c>
-      <c r="E87" s="7">
-        <v>1</v>
-      </c>
-      <c r="F87" s="8">
+      <c r="E87" s="6">
+        <v>1</v>
+      </c>
+      <c r="F87" s="7">
         <f>VLOOKUP(D87,'Final Data'!$G:$J,3,FALSE)</f>
         <v>162443</v>
       </c>
-      <c r="G87" s="8">
+      <c r="G87" s="7">
         <f>VLOOKUP(D87,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11962</v>
       </c>
@@ -12344,21 +12351,21 @@
       <c r="A88" t="s">
         <v>368</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B88" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A88)</f>
         <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>257</v>
       </c>
-      <c r="E88" s="7">
-        <v>1</v>
-      </c>
-      <c r="F88" s="8">
+      <c r="E88" s="6">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7">
         <f>VLOOKUP(D88,'Final Data'!$G:$J,3,FALSE)</f>
         <v>136094</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88" s="7">
         <f>VLOOKUP(D88,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7210</v>
       </c>
@@ -12367,21 +12374,21 @@
       <c r="A89" t="s">
         <v>369</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A89)</f>
         <v>1</v>
       </c>
       <c r="D89" t="s">
         <v>268</v>
       </c>
-      <c r="E89" s="7">
-        <v>1</v>
-      </c>
-      <c r="F89" s="8">
+      <c r="E89" s="6">
+        <v>1</v>
+      </c>
+      <c r="F89" s="7">
         <f>VLOOKUP(D89,'Final Data'!$G:$J,3,FALSE)</f>
         <v>138920</v>
       </c>
-      <c r="G89" s="8">
+      <c r="G89" s="7">
         <f>VLOOKUP(D89,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11428</v>
       </c>
@@ -12390,21 +12397,21 @@
       <c r="A90" t="s">
         <v>373</v>
       </c>
-      <c r="B90" s="7">
+      <c r="B90" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A90)</f>
         <v>1</v>
       </c>
       <c r="D90" t="s">
         <v>272</v>
       </c>
-      <c r="E90" s="7">
-        <v>1</v>
-      </c>
-      <c r="F90" s="8">
+      <c r="E90" s="6">
+        <v>1</v>
+      </c>
+      <c r="F90" s="7">
         <f>VLOOKUP(D90,'Final Data'!$G:$J,3,FALSE)</f>
         <v>73415</v>
       </c>
-      <c r="G90" s="8">
+      <c r="G90" s="7">
         <f>VLOOKUP(D90,'Final Data'!$G:$J,4,FALSE)</f>
         <v>89206</v>
       </c>
@@ -12413,21 +12420,21 @@
       <c r="A91" t="s">
         <v>376</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A91)</f>
         <v>1</v>
       </c>
       <c r="D91" t="s">
         <v>275</v>
       </c>
-      <c r="E91" s="7">
-        <v>1</v>
-      </c>
-      <c r="F91" s="8">
+      <c r="E91" s="6">
+        <v>1</v>
+      </c>
+      <c r="F91" s="7">
         <f>VLOOKUP(D91,'Final Data'!$G:$J,3,FALSE)</f>
         <v>68655</v>
       </c>
-      <c r="G91" s="8">
+      <c r="G91" s="7">
         <f>VLOOKUP(D91,'Final Data'!$G:$J,4,FALSE)</f>
         <v>14557</v>
       </c>
@@ -12436,21 +12443,21 @@
       <c r="A92" t="s">
         <v>380</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A92)</f>
         <v>2</v>
       </c>
       <c r="D92" t="s">
         <v>276</v>
       </c>
-      <c r="E92" s="7">
-        <v>1</v>
-      </c>
-      <c r="F92" s="8">
+      <c r="E92" s="6">
+        <v>1</v>
+      </c>
+      <c r="F92" s="7">
         <f>VLOOKUP(D92,'Final Data'!$G:$J,3,FALSE)</f>
         <v>87800</v>
       </c>
-      <c r="G92" s="8">
+      <c r="G92" s="7">
         <f>VLOOKUP(D92,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12205</v>
       </c>
@@ -12459,21 +12466,21 @@
       <c r="A93" t="s">
         <v>385</v>
       </c>
-      <c r="B93" s="7">
+      <c r="B93" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A93)</f>
         <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>278</v>
       </c>
-      <c r="E93" s="7">
-        <v>1</v>
-      </c>
-      <c r="F93" s="8">
+      <c r="E93" s="6">
+        <v>1</v>
+      </c>
+      <c r="F93" s="7">
         <f>VLOOKUP(D93,'Final Data'!$G:$J,3,FALSE)</f>
         <v>119542</v>
       </c>
-      <c r="G93" s="8">
+      <c r="G93" s="7">
         <f>VLOOKUP(D93,'Final Data'!$G:$J,4,FALSE)</f>
         <v>39712</v>
       </c>
@@ -12482,21 +12489,21 @@
       <c r="A94" t="s">
         <v>388</v>
       </c>
-      <c r="B94" s="7">
+      <c r="B94" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A94)</f>
         <v>2</v>
       </c>
       <c r="D94" t="s">
         <v>282</v>
       </c>
-      <c r="E94" s="7">
-        <v>1</v>
-      </c>
-      <c r="F94" s="8">
+      <c r="E94" s="6">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7">
         <f>VLOOKUP(D94,'Final Data'!$G:$J,3,FALSE)</f>
         <v>124844</v>
       </c>
-      <c r="G94" s="8">
+      <c r="G94" s="7">
         <f>VLOOKUP(D94,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10520</v>
       </c>
@@ -12505,21 +12512,21 @@
       <c r="A95" t="s">
         <v>393</v>
       </c>
-      <c r="B95" s="7">
+      <c r="B95" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A95)</f>
         <v>1</v>
       </c>
       <c r="D95" t="s">
         <v>295</v>
       </c>
-      <c r="E95" s="7">
-        <v>1</v>
-      </c>
-      <c r="F95" s="8">
+      <c r="E95" s="6">
+        <v>1</v>
+      </c>
+      <c r="F95" s="7">
         <f>VLOOKUP(D95,'Final Data'!$G:$J,3,FALSE)</f>
         <v>100305</v>
       </c>
-      <c r="G95" s="8">
+      <c r="G95" s="7">
         <f>VLOOKUP(D95,'Final Data'!$G:$J,4,FALSE)</f>
         <v>52076</v>
       </c>
@@ -12528,21 +12535,21 @@
       <c r="A96" t="s">
         <v>396</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A96)</f>
         <v>1</v>
       </c>
       <c r="D96" t="s">
         <v>298</v>
       </c>
-      <c r="E96" s="7">
-        <v>1</v>
-      </c>
-      <c r="F96" s="11">
+      <c r="E96" s="6">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10">
         <f>VLOOKUP(D96,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G96" s="11">
+      <c r="G96" s="10">
         <f>VLOOKUP(D96,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12551,21 +12558,21 @@
       <c r="A97" t="s">
         <v>399</v>
       </c>
-      <c r="B97" s="7">
+      <c r="B97" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A97)</f>
         <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>314</v>
       </c>
-      <c r="E97" s="7">
-        <v>1</v>
-      </c>
-      <c r="F97" s="8">
+      <c r="E97" s="6">
+        <v>1</v>
+      </c>
+      <c r="F97" s="7">
         <f>VLOOKUP(D97,'Final Data'!$G:$J,3,FALSE)</f>
         <v>108281</v>
       </c>
-      <c r="G97" s="8">
+      <c r="G97" s="7">
         <f>VLOOKUP(D97,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8235</v>
       </c>
@@ -12574,21 +12581,21 @@
       <c r="A98" t="s">
         <v>404</v>
       </c>
-      <c r="B98" s="7">
+      <c r="B98" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A98)</f>
         <v>4</v>
       </c>
       <c r="D98" t="s">
         <v>318</v>
       </c>
-      <c r="E98" s="7">
-        <v>1</v>
-      </c>
-      <c r="F98" s="8">
+      <c r="E98" s="6">
+        <v>1</v>
+      </c>
+      <c r="F98" s="7">
         <f>VLOOKUP(D98,'Final Data'!$G:$J,3,FALSE)</f>
         <v>45321</v>
       </c>
-      <c r="G98" s="8">
+      <c r="G98" s="7">
         <f>VLOOKUP(D98,'Final Data'!$G:$J,4,FALSE)</f>
         <v>99467</v>
       </c>
@@ -12597,21 +12604,21 @@
       <c r="A99" t="s">
         <v>415</v>
       </c>
-      <c r="B99" s="7">
+      <c r="B99" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A99)</f>
         <v>1</v>
       </c>
       <c r="D99" t="s">
         <v>330</v>
       </c>
-      <c r="E99" s="7">
-        <v>1</v>
-      </c>
-      <c r="F99" s="11">
+      <c r="E99" s="6">
+        <v>1</v>
+      </c>
+      <c r="F99" s="10">
         <f>VLOOKUP(D99,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G99" s="11">
+      <c r="G99" s="10">
         <f>VLOOKUP(D99,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12620,21 +12627,21 @@
       <c r="A100" t="s">
         <v>416</v>
       </c>
-      <c r="B100" s="7">
+      <c r="B100" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A100)</f>
         <v>2</v>
       </c>
       <c r="D100" t="s">
         <v>331</v>
       </c>
-      <c r="E100" s="7">
-        <v>1</v>
-      </c>
-      <c r="F100" s="8">
+      <c r="E100" s="6">
+        <v>1</v>
+      </c>
+      <c r="F100" s="7">
         <f>VLOOKUP(D100,'Final Data'!$G:$J,3,FALSE)</f>
         <v>66538</v>
       </c>
-      <c r="G100" s="8">
+      <c r="G100" s="7">
         <f>VLOOKUP(D100,'Final Data'!$G:$J,4,FALSE)</f>
         <v>42230</v>
       </c>
@@ -12643,21 +12650,21 @@
       <c r="A101" t="s">
         <v>423</v>
       </c>
-      <c r="B101" s="7">
+      <c r="B101" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A101)</f>
         <v>1</v>
       </c>
       <c r="D101" t="s">
         <v>336</v>
       </c>
-      <c r="E101" s="7">
-        <v>1</v>
-      </c>
-      <c r="F101" s="8">
+      <c r="E101" s="6">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7">
         <f>VLOOKUP(D101,'Final Data'!$G:$J,3,FALSE)</f>
         <v>61341</v>
       </c>
-      <c r="G101" s="8">
+      <c r="G101" s="7">
         <f>VLOOKUP(D101,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10942</v>
       </c>
@@ -12666,21 +12673,21 @@
       <c r="A102" t="s">
         <v>426</v>
       </c>
-      <c r="B102" s="7">
+      <c r="B102" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A102)</f>
         <v>4</v>
       </c>
       <c r="D102" t="s">
         <v>337</v>
       </c>
-      <c r="E102" s="7">
-        <v>1</v>
-      </c>
-      <c r="F102" s="8">
+      <c r="E102" s="6">
+        <v>1</v>
+      </c>
+      <c r="F102" s="7">
         <f>VLOOKUP(D102,'Final Data'!$G:$J,3,FALSE)</f>
         <v>153381</v>
       </c>
-      <c r="G102" s="8">
+      <c r="G102" s="7">
         <f>VLOOKUP(D102,'Final Data'!$G:$J,4,FALSE)</f>
         <v>29955</v>
       </c>
@@ -12689,21 +12696,21 @@
       <c r="A103" t="s">
         <v>435</v>
       </c>
-      <c r="B103" s="7">
+      <c r="B103" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A103)</f>
         <v>2</v>
       </c>
       <c r="D103" t="s">
         <v>339</v>
       </c>
-      <c r="E103" s="7">
-        <v>1</v>
-      </c>
-      <c r="F103" s="8">
+      <c r="E103" s="6">
+        <v>1</v>
+      </c>
+      <c r="F103" s="7">
         <f>VLOOKUP(D103,'Final Data'!$G:$J,3,FALSE)</f>
         <v>127948</v>
       </c>
-      <c r="G103" s="8">
+      <c r="G103" s="7">
         <f>VLOOKUP(D103,'Final Data'!$G:$J,4,FALSE)</f>
         <v>16080</v>
       </c>
@@ -12712,21 +12719,21 @@
       <c r="A104" t="s">
         <v>441</v>
       </c>
-      <c r="B104" s="7">
+      <c r="B104" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A104)</f>
         <v>2</v>
       </c>
       <c r="D104" t="s">
         <v>343</v>
       </c>
-      <c r="E104" s="7">
-        <v>1</v>
-      </c>
-      <c r="F104" s="8">
+      <c r="E104" s="6">
+        <v>1</v>
+      </c>
+      <c r="F104" s="7">
         <f>VLOOKUP(D104,'Final Data'!$G:$J,3,FALSE)</f>
         <v>107215</v>
       </c>
-      <c r="G104" s="8">
+      <c r="G104" s="7">
         <f>VLOOKUP(D104,'Final Data'!$G:$J,4,FALSE)</f>
         <v>26581</v>
       </c>
@@ -12735,21 +12742,21 @@
       <c r="A105" t="s">
         <v>447</v>
       </c>
-      <c r="B105" s="7">
+      <c r="B105" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A105)</f>
         <v>1</v>
       </c>
       <c r="D105" t="s">
         <v>346</v>
       </c>
-      <c r="E105" s="7">
-        <v>1</v>
-      </c>
-      <c r="F105" s="11">
+      <c r="E105" s="6">
+        <v>1</v>
+      </c>
+      <c r="F105" s="10">
         <f>VLOOKUP(D105,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G105" s="11">
+      <c r="G105" s="10">
         <f>VLOOKUP(D105,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12758,21 +12765,21 @@
       <c r="A106" t="s">
         <v>448</v>
       </c>
-      <c r="B106" s="7">
+      <c r="B106" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A106)</f>
         <v>1</v>
       </c>
       <c r="D106" t="s">
         <v>349</v>
       </c>
-      <c r="E106" s="7">
-        <v>1</v>
-      </c>
-      <c r="F106" s="8">
+      <c r="E106" s="6">
+        <v>1</v>
+      </c>
+      <c r="F106" s="7">
         <f>VLOOKUP(D106,'Final Data'!$G:$J,3,FALSE)</f>
         <v>109326</v>
       </c>
-      <c r="G106" s="8">
+      <c r="G106" s="7">
         <f>VLOOKUP(D106,'Final Data'!$G:$J,4,FALSE)</f>
         <v>40096</v>
       </c>
@@ -12781,21 +12788,21 @@
       <c r="A107" t="s">
         <v>452</v>
       </c>
-      <c r="B107" s="7">
+      <c r="B107" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A107)</f>
         <v>1</v>
       </c>
       <c r="D107" t="s">
         <v>352</v>
       </c>
-      <c r="E107" s="7">
-        <v>1</v>
-      </c>
-      <c r="F107" s="8">
+      <c r="E107" s="6">
+        <v>1</v>
+      </c>
+      <c r="F107" s="7">
         <f>VLOOKUP(D107,'Final Data'!$G:$J,3,FALSE)</f>
         <v>69896</v>
       </c>
-      <c r="G107" s="8">
+      <c r="G107" s="7">
         <f>VLOOKUP(D107,'Final Data'!$G:$J,4,FALSE)</f>
         <v>6200</v>
       </c>
@@ -12804,21 +12811,21 @@
       <c r="A108" t="s">
         <v>453</v>
       </c>
-      <c r="B108" s="7">
+      <c r="B108" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A108)</f>
         <v>1</v>
       </c>
       <c r="D108" t="s">
         <v>353</v>
       </c>
-      <c r="E108" s="7">
-        <v>1</v>
-      </c>
-      <c r="F108" s="8">
+      <c r="E108" s="6">
+        <v>1</v>
+      </c>
+      <c r="F108" s="7">
         <f>VLOOKUP(D108,'Final Data'!$G:$J,3,FALSE)</f>
         <v>86149</v>
       </c>
-      <c r="G108" s="8">
+      <c r="G108" s="7">
         <f>VLOOKUP(D108,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8898</v>
       </c>
@@ -12827,21 +12834,21 @@
       <c r="A109" t="s">
         <v>457</v>
       </c>
-      <c r="B109" s="7">
+      <c r="B109" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A109)</f>
         <v>1</v>
       </c>
       <c r="D109" t="s">
         <v>359</v>
       </c>
-      <c r="E109" s="7">
-        <v>1</v>
-      </c>
-      <c r="F109" s="11">
+      <c r="E109" s="6">
+        <v>1</v>
+      </c>
+      <c r="F109" s="10">
         <f>VLOOKUP(D109,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G109" s="11">
+      <c r="G109" s="10">
         <f>VLOOKUP(D109,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -12850,21 +12857,21 @@
       <c r="A110" t="s">
         <v>460</v>
       </c>
-      <c r="B110" s="7">
+      <c r="B110" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A110)</f>
         <v>1</v>
       </c>
       <c r="D110" t="s">
         <v>360</v>
       </c>
-      <c r="E110" s="7">
-        <v>1</v>
-      </c>
-      <c r="F110" s="8">
+      <c r="E110" s="6">
+        <v>1</v>
+      </c>
+      <c r="F110" s="7">
         <f>VLOOKUP(D110,'Final Data'!$G:$J,3,FALSE)</f>
         <v>113469</v>
       </c>
-      <c r="G110" s="8">
+      <c r="G110" s="7">
         <f>VLOOKUP(D110,'Final Data'!$G:$J,4,FALSE)</f>
         <v>23353</v>
       </c>
@@ -12873,21 +12880,21 @@
       <c r="A111" t="s">
         <v>461</v>
       </c>
-      <c r="B111" s="7">
+      <c r="B111" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A111)</f>
         <v>1</v>
       </c>
       <c r="D111" t="s">
         <v>365</v>
       </c>
-      <c r="E111" s="7">
-        <v>1</v>
-      </c>
-      <c r="F111" s="8">
+      <c r="E111" s="6">
+        <v>1</v>
+      </c>
+      <c r="F111" s="7">
         <f>VLOOKUP(D111,'Final Data'!$G:$J,3,FALSE)</f>
         <v>105035</v>
       </c>
-      <c r="G111" s="8">
+      <c r="G111" s="7">
         <f>VLOOKUP(D111,'Final Data'!$G:$J,4,FALSE)</f>
         <v>65952</v>
       </c>
@@ -12896,21 +12903,21 @@
       <c r="A112" t="s">
         <v>463</v>
       </c>
-      <c r="B112" s="7">
+      <c r="B112" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A112)</f>
         <v>5</v>
       </c>
       <c r="D112" t="s">
         <v>368</v>
       </c>
-      <c r="E112" s="7">
-        <v>1</v>
-      </c>
-      <c r="F112" s="8">
+      <c r="E112" s="6">
+        <v>1</v>
+      </c>
+      <c r="F112" s="7">
         <f>VLOOKUP(D112,'Final Data'!$G:$J,3,FALSE)</f>
         <v>105313</v>
       </c>
-      <c r="G112" s="8">
+      <c r="G112" s="7">
         <f>VLOOKUP(D112,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7336</v>
       </c>
@@ -12919,21 +12926,21 @@
       <c r="A113" t="s">
         <v>476</v>
       </c>
-      <c r="B113" s="7">
+      <c r="B113" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A113)</f>
         <v>1</v>
       </c>
       <c r="D113" t="s">
         <v>369</v>
       </c>
-      <c r="E113" s="7">
-        <v>1</v>
-      </c>
-      <c r="F113" s="8">
+      <c r="E113" s="6">
+        <v>1</v>
+      </c>
+      <c r="F113" s="7">
         <f>VLOOKUP(D113,'Final Data'!$G:$J,3,FALSE)</f>
         <v>202862</v>
       </c>
-      <c r="G113" s="8">
+      <c r="G113" s="7">
         <f>VLOOKUP(D113,'Final Data'!$G:$J,4,FALSE)</f>
         <v>20387</v>
       </c>
@@ -12942,21 +12949,21 @@
       <c r="A114" t="s">
         <v>480</v>
       </c>
-      <c r="B114" s="7">
+      <c r="B114" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A114)</f>
         <v>1</v>
       </c>
       <c r="D114" t="s">
         <v>373</v>
       </c>
-      <c r="E114" s="7">
-        <v>1</v>
-      </c>
-      <c r="F114" s="8">
+      <c r="E114" s="6">
+        <v>1</v>
+      </c>
+      <c r="F114" s="7">
         <f>VLOOKUP(D114,'Final Data'!$G:$J,3,FALSE)</f>
         <v>99704</v>
       </c>
-      <c r="G114" s="8">
+      <c r="G114" s="7">
         <f>VLOOKUP(D114,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7069</v>
       </c>
@@ -12965,21 +12972,21 @@
       <c r="A115" t="s">
         <v>483</v>
       </c>
-      <c r="B115" s="7">
+      <c r="B115" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A115)</f>
         <v>1</v>
       </c>
       <c r="D115" t="s">
         <v>376</v>
       </c>
-      <c r="E115" s="7">
-        <v>1</v>
-      </c>
-      <c r="F115" s="8">
+      <c r="E115" s="6">
+        <v>1</v>
+      </c>
+      <c r="F115" s="7">
         <f>VLOOKUP(D115,'Final Data'!$G:$J,3,FALSE)</f>
         <v>49950</v>
       </c>
-      <c r="G115" s="8">
+      <c r="G115" s="7">
         <f>VLOOKUP(D115,'Final Data'!$G:$J,4,FALSE)</f>
         <v>28235</v>
       </c>
@@ -12988,21 +12995,21 @@
       <c r="A116" t="s">
         <v>486</v>
       </c>
-      <c r="B116" s="7">
+      <c r="B116" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A116)</f>
         <v>1</v>
       </c>
       <c r="D116" t="s">
         <v>385</v>
       </c>
-      <c r="E116" s="7">
-        <v>1</v>
-      </c>
-      <c r="F116" s="8">
+      <c r="E116" s="6">
+        <v>1</v>
+      </c>
+      <c r="F116" s="7">
         <f>VLOOKUP(D116,'Final Data'!$G:$J,3,FALSE)</f>
         <v>120060</v>
       </c>
-      <c r="G116" s="8">
+      <c r="G116" s="7">
         <f>VLOOKUP(D116,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8440</v>
       </c>
@@ -13011,21 +13018,21 @@
       <c r="A117" t="s">
         <v>489</v>
       </c>
-      <c r="B117" s="7">
+      <c r="B117" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A117)</f>
         <v>3</v>
       </c>
       <c r="D117" t="s">
         <v>393</v>
       </c>
-      <c r="E117" s="7">
-        <v>1</v>
-      </c>
-      <c r="F117" s="11">
+      <c r="E117" s="6">
+        <v>1</v>
+      </c>
+      <c r="F117" s="10">
         <f>VLOOKUP(D117,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G117" s="11">
+      <c r="G117" s="10">
         <f>VLOOKUP(D117,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13034,21 +13041,21 @@
       <c r="A118" t="s">
         <v>496</v>
       </c>
-      <c r="B118" s="7">
+      <c r="B118" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A118)</f>
         <v>3</v>
       </c>
       <c r="D118" t="s">
         <v>396</v>
       </c>
-      <c r="E118" s="7">
-        <v>1</v>
-      </c>
-      <c r="F118" s="8">
+      <c r="E118" s="6">
+        <v>1</v>
+      </c>
+      <c r="F118" s="7">
         <f>VLOOKUP(D118,'Final Data'!$G:$J,3,FALSE)</f>
         <v>125229</v>
       </c>
-      <c r="G118" s="8">
+      <c r="G118" s="7">
         <f>VLOOKUP(D118,'Final Data'!$G:$J,4,FALSE)</f>
         <v>5605</v>
       </c>
@@ -13057,21 +13064,21 @@
       <c r="A119" t="s">
         <v>504</v>
       </c>
-      <c r="B119" s="7">
+      <c r="B119" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A119)</f>
         <v>1</v>
       </c>
       <c r="D119" t="s">
         <v>415</v>
       </c>
-      <c r="E119" s="7">
-        <v>1</v>
-      </c>
-      <c r="F119" s="8">
+      <c r="E119" s="6">
+        <v>1</v>
+      </c>
+      <c r="F119" s="7">
         <f>VLOOKUP(D119,'Final Data'!$G:$J,3,FALSE)</f>
         <v>67836</v>
       </c>
-      <c r="G119" s="8">
+      <c r="G119" s="7">
         <f>VLOOKUP(D119,'Final Data'!$G:$J,4,FALSE)</f>
         <v>27728</v>
       </c>
@@ -13080,21 +13087,21 @@
       <c r="A120" t="s">
         <v>505</v>
       </c>
-      <c r="B120" s="7">
+      <c r="B120" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A120)</f>
         <v>1</v>
       </c>
       <c r="D120" t="s">
         <v>423</v>
       </c>
-      <c r="E120" s="7">
-        <v>1</v>
-      </c>
-      <c r="F120" s="8">
+      <c r="E120" s="6">
+        <v>1</v>
+      </c>
+      <c r="F120" s="7">
         <f>VLOOKUP(D120,'Final Data'!$G:$J,3,FALSE)</f>
         <v>129638</v>
       </c>
-      <c r="G120" s="8">
+      <c r="G120" s="7">
         <f>VLOOKUP(D120,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12716</v>
       </c>
@@ -13103,21 +13110,21 @@
       <c r="A121" t="s">
         <v>508</v>
       </c>
-      <c r="B121" s="7">
+      <c r="B121" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A121)</f>
         <v>2</v>
       </c>
       <c r="D121" t="s">
         <v>447</v>
       </c>
-      <c r="E121" s="7">
-        <v>1</v>
-      </c>
-      <c r="F121" s="8">
+      <c r="E121" s="6">
+        <v>1</v>
+      </c>
+      <c r="F121" s="7">
         <f>VLOOKUP(D121,'Final Data'!$G:$J,3,FALSE)</f>
         <v>92650</v>
       </c>
-      <c r="G121" s="8">
+      <c r="G121" s="7">
         <f>VLOOKUP(D121,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4872</v>
       </c>
@@ -13126,21 +13133,21 @@
       <c r="A122" t="s">
         <v>514</v>
       </c>
-      <c r="B122" s="7">
+      <c r="B122" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A122)</f>
         <v>2</v>
       </c>
       <c r="D122" t="s">
         <v>448</v>
       </c>
-      <c r="E122" s="7">
-        <v>1</v>
-      </c>
-      <c r="F122" s="8">
+      <c r="E122" s="6">
+        <v>1</v>
+      </c>
+      <c r="F122" s="7">
         <f>VLOOKUP(D122,'Final Data'!$G:$J,3,FALSE)</f>
         <v>93691</v>
       </c>
-      <c r="G122" s="8">
+      <c r="G122" s="7">
         <f>VLOOKUP(D122,'Final Data'!$G:$J,4,FALSE)</f>
         <v>28829</v>
       </c>
@@ -13149,21 +13156,21 @@
       <c r="A123" t="s">
         <v>518</v>
       </c>
-      <c r="B123" s="7">
+      <c r="B123" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A123)</f>
         <v>1</v>
       </c>
       <c r="D123" t="s">
         <v>452</v>
       </c>
-      <c r="E123" s="7">
-        <v>1</v>
-      </c>
-      <c r="F123" s="11">
+      <c r="E123" s="6">
+        <v>1</v>
+      </c>
+      <c r="F123" s="10">
         <f>VLOOKUP(D123,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G123" s="11">
+      <c r="G123" s="10">
         <f>VLOOKUP(D123,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13172,21 +13179,21 @@
       <c r="A124" t="s">
         <v>522</v>
       </c>
-      <c r="B124" s="7">
+      <c r="B124" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A124)</f>
         <v>2</v>
       </c>
       <c r="D124" t="s">
         <v>453</v>
       </c>
-      <c r="E124" s="7">
-        <v>1</v>
-      </c>
-      <c r="F124" s="8">
+      <c r="E124" s="6">
+        <v>1</v>
+      </c>
+      <c r="F124" s="7">
         <f>VLOOKUP(D124,'Final Data'!$G:$J,3,FALSE)</f>
         <v>112944</v>
       </c>
-      <c r="G124" s="8">
+      <c r="G124" s="7">
         <f>VLOOKUP(D124,'Final Data'!$G:$J,4,FALSE)</f>
         <v>13145</v>
       </c>
@@ -13195,21 +13202,21 @@
       <c r="A125" t="s">
         <v>525</v>
       </c>
-      <c r="B125" s="7">
+      <c r="B125" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A125)</f>
         <v>1</v>
       </c>
       <c r="D125" t="s">
         <v>457</v>
       </c>
-      <c r="E125" s="7">
-        <v>1</v>
-      </c>
-      <c r="F125" s="8">
+      <c r="E125" s="6">
+        <v>1</v>
+      </c>
+      <c r="F125" s="7">
         <f>VLOOKUP(D125,'Final Data'!$G:$J,3,FALSE)</f>
         <v>72715</v>
       </c>
-      <c r="G125" s="8">
+      <c r="G125" s="7">
         <f>VLOOKUP(D125,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11328</v>
       </c>
@@ -13218,21 +13225,21 @@
       <c r="A126" t="s">
         <v>531</v>
       </c>
-      <c r="B126" s="7">
+      <c r="B126" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A126)</f>
         <v>1</v>
       </c>
       <c r="D126" t="s">
         <v>460</v>
       </c>
-      <c r="E126" s="7">
-        <v>1</v>
-      </c>
-      <c r="F126" s="8">
+      <c r="E126" s="6">
+        <v>1</v>
+      </c>
+      <c r="F126" s="7">
         <f>VLOOKUP(D126,'Final Data'!$G:$J,3,FALSE)</f>
         <v>88540</v>
       </c>
-      <c r="G126" s="8">
+      <c r="G126" s="7">
         <f>VLOOKUP(D126,'Final Data'!$G:$J,4,FALSE)</f>
         <v>66880</v>
       </c>
@@ -13241,21 +13248,21 @@
       <c r="A127" t="s">
         <v>534</v>
       </c>
-      <c r="B127" s="7">
+      <c r="B127" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A127)</f>
         <v>1</v>
       </c>
       <c r="D127" t="s">
         <v>461</v>
       </c>
-      <c r="E127" s="7">
-        <v>1</v>
-      </c>
-      <c r="F127" s="8">
+      <c r="E127" s="6">
+        <v>1</v>
+      </c>
+      <c r="F127" s="7">
         <f>VLOOKUP(D127,'Final Data'!$G:$J,3,FALSE)</f>
         <v>141185</v>
       </c>
-      <c r="G127" s="8">
+      <c r="G127" s="7">
         <f>VLOOKUP(D127,'Final Data'!$G:$J,4,FALSE)</f>
         <v>5999</v>
       </c>
@@ -13264,21 +13271,21 @@
       <c r="A128" t="s">
         <v>537</v>
       </c>
-      <c r="B128" s="7">
+      <c r="B128" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A128)</f>
         <v>3</v>
       </c>
       <c r="D128" t="s">
         <v>476</v>
       </c>
-      <c r="E128" s="7">
-        <v>1</v>
-      </c>
-      <c r="F128" s="8">
+      <c r="E128" s="6">
+        <v>1</v>
+      </c>
+      <c r="F128" s="7">
         <f>VLOOKUP(D128,'Final Data'!$G:$J,3,FALSE)</f>
         <v>106875</v>
       </c>
-      <c r="G128" s="8">
+      <c r="G128" s="7">
         <f>VLOOKUP(D128,'Final Data'!$G:$J,4,FALSE)</f>
         <v>8905</v>
       </c>
@@ -13287,21 +13294,21 @@
       <c r="A129" t="s">
         <v>542</v>
       </c>
-      <c r="B129" s="7">
+      <c r="B129" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A129)</f>
         <v>1</v>
       </c>
       <c r="D129" t="s">
         <v>480</v>
       </c>
-      <c r="E129" s="7">
-        <v>1</v>
-      </c>
-      <c r="F129" s="8">
+      <c r="E129" s="6">
+        <v>1</v>
+      </c>
+      <c r="F129" s="7">
         <f>VLOOKUP(D129,'Final Data'!$G:$J,3,FALSE)</f>
         <v>121667</v>
       </c>
-      <c r="G129" s="8">
+      <c r="G129" s="7">
         <f>VLOOKUP(D129,'Final Data'!$G:$J,4,FALSE)</f>
         <v>2591</v>
       </c>
@@ -13310,21 +13317,21 @@
       <c r="A130" t="s">
         <v>546</v>
       </c>
-      <c r="B130" s="7">
+      <c r="B130" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A130)</f>
         <v>1</v>
       </c>
       <c r="D130" t="s">
         <v>483</v>
       </c>
-      <c r="E130" s="7">
-        <v>1</v>
-      </c>
-      <c r="F130" s="8">
+      <c r="E130" s="6">
+        <v>1</v>
+      </c>
+      <c r="F130" s="7">
         <f>VLOOKUP(D130,'Final Data'!$G:$J,3,FALSE)</f>
         <v>37188</v>
       </c>
-      <c r="G130" s="8">
+      <c r="G130" s="7">
         <f>VLOOKUP(D130,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4917</v>
       </c>
@@ -13333,21 +13340,21 @@
       <c r="A131" t="s">
         <v>547</v>
       </c>
-      <c r="B131" s="7">
+      <c r="B131" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A131)</f>
         <v>1</v>
       </c>
       <c r="D131" t="s">
         <v>486</v>
       </c>
-      <c r="E131" s="7">
-        <v>1</v>
-      </c>
-      <c r="F131" s="11">
+      <c r="E131" s="6">
+        <v>1</v>
+      </c>
+      <c r="F131" s="10">
         <f>VLOOKUP(D131,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G131" s="11">
+      <c r="G131" s="10">
         <f>VLOOKUP(D131,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13356,21 +13363,21 @@
       <c r="A132" t="s">
         <v>553</v>
       </c>
-      <c r="B132" s="7">
+      <c r="B132" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A132)</f>
         <v>2</v>
       </c>
       <c r="D132" t="s">
         <v>504</v>
       </c>
-      <c r="E132" s="7">
-        <v>1</v>
-      </c>
-      <c r="F132" s="11">
+      <c r="E132" s="6">
+        <v>1</v>
+      </c>
+      <c r="F132" s="10">
         <f>VLOOKUP(D132,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G132" s="11">
+      <c r="G132" s="10">
         <f>VLOOKUP(D132,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13379,21 +13386,21 @@
       <c r="A133" t="s">
         <v>560</v>
       </c>
-      <c r="B133" s="7">
+      <c r="B133" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A133)</f>
         <v>2</v>
       </c>
       <c r="D133" t="s">
         <v>505</v>
       </c>
-      <c r="E133" s="7">
-        <v>1</v>
-      </c>
-      <c r="F133" s="8">
+      <c r="E133" s="6">
+        <v>1</v>
+      </c>
+      <c r="F133" s="7">
         <f>VLOOKUP(D133,'Final Data'!$G:$J,3,FALSE)</f>
         <v>92952</v>
       </c>
-      <c r="G133" s="8">
+      <c r="G133" s="7">
         <f>VLOOKUP(D133,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11205</v>
       </c>
@@ -13402,21 +13409,21 @@
       <c r="A134" t="s">
         <v>565</v>
       </c>
-      <c r="B134" s="7">
+      <c r="B134" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A134)</f>
         <v>1</v>
       </c>
       <c r="D134" t="s">
         <v>518</v>
       </c>
-      <c r="E134" s="7">
-        <v>1</v>
-      </c>
-      <c r="F134" s="8">
+      <c r="E134" s="6">
+        <v>1</v>
+      </c>
+      <c r="F134" s="7">
         <f>VLOOKUP(D134,'Final Data'!$G:$J,3,FALSE)</f>
         <v>75114</v>
       </c>
-      <c r="G134" s="8">
+      <c r="G134" s="7">
         <f>VLOOKUP(D134,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12220</v>
       </c>
@@ -13425,21 +13432,21 @@
       <c r="A135" t="s">
         <v>566</v>
       </c>
-      <c r="B135" s="7">
+      <c r="B135" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A135)</f>
         <v>1</v>
       </c>
       <c r="D135" t="s">
         <v>525</v>
       </c>
-      <c r="E135" s="7">
-        <v>1</v>
-      </c>
-      <c r="F135" s="11">
+      <c r="E135" s="6">
+        <v>1</v>
+      </c>
+      <c r="F135" s="10">
         <f>VLOOKUP(D135,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G135" s="11">
+      <c r="G135" s="10">
         <f>VLOOKUP(D135,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13448,21 +13455,21 @@
       <c r="A136" t="s">
         <v>571</v>
       </c>
-      <c r="B136" s="7">
+      <c r="B136" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A136)</f>
         <v>2</v>
       </c>
       <c r="D136" t="s">
         <v>531</v>
       </c>
-      <c r="E136" s="7">
-        <v>1</v>
-      </c>
-      <c r="F136" s="8">
+      <c r="E136" s="6">
+        <v>1</v>
+      </c>
+      <c r="F136" s="7">
         <f>VLOOKUP(D136,'Final Data'!$G:$J,3,FALSE)</f>
         <v>100602</v>
       </c>
-      <c r="G136" s="8">
+      <c r="G136" s="7">
         <f>VLOOKUP(D136,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4238</v>
       </c>
@@ -13471,21 +13478,21 @@
       <c r="A137" t="s">
         <v>574</v>
       </c>
-      <c r="B137" s="7">
+      <c r="B137" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A137)</f>
         <v>1</v>
       </c>
       <c r="D137" t="s">
         <v>534</v>
       </c>
-      <c r="E137" s="7">
-        <v>1</v>
-      </c>
-      <c r="F137" s="8">
+      <c r="E137" s="6">
+        <v>1</v>
+      </c>
+      <c r="F137" s="7">
         <f>VLOOKUP(D137,'Final Data'!$G:$J,3,FALSE)</f>
         <v>60885</v>
       </c>
-      <c r="G137" s="8">
+      <c r="G137" s="7">
         <f>VLOOKUP(D137,'Final Data'!$G:$J,4,FALSE)</f>
         <v>7969</v>
       </c>
@@ -13494,21 +13501,21 @@
       <c r="A138" t="s">
         <v>577</v>
       </c>
-      <c r="B138" s="7">
+      <c r="B138" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A138)</f>
         <v>1</v>
       </c>
       <c r="D138" t="s">
         <v>542</v>
       </c>
-      <c r="E138" s="7">
-        <v>1</v>
-      </c>
-      <c r="F138" s="8">
+      <c r="E138" s="6">
+        <v>1</v>
+      </c>
+      <c r="F138" s="7">
         <f>VLOOKUP(D138,'Final Data'!$G:$J,3,FALSE)</f>
         <v>110208</v>
       </c>
-      <c r="G138" s="8">
+      <c r="G138" s="7">
         <f>VLOOKUP(D138,'Final Data'!$G:$J,4,FALSE)</f>
         <v>5907</v>
       </c>
@@ -13517,21 +13524,21 @@
       <c r="A139" t="s">
         <v>583</v>
       </c>
-      <c r="B139" s="7">
+      <c r="B139" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A139)</f>
         <v>1</v>
       </c>
       <c r="D139" t="s">
         <v>546</v>
       </c>
-      <c r="E139" s="7">
-        <v>1</v>
-      </c>
-      <c r="F139" s="8">
+      <c r="E139" s="6">
+        <v>1</v>
+      </c>
+      <c r="F139" s="7">
         <f>VLOOKUP(D139,'Final Data'!$G:$J,3,FALSE)</f>
         <v>93787</v>
       </c>
-      <c r="G139" s="8">
+      <c r="G139" s="7">
         <f>VLOOKUP(D139,'Final Data'!$G:$J,4,FALSE)</f>
         <v>18622</v>
       </c>
@@ -13540,21 +13547,21 @@
       <c r="A140" t="s">
         <v>586</v>
       </c>
-      <c r="B140" s="7">
+      <c r="B140" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A140)</f>
         <v>2</v>
       </c>
       <c r="D140" t="s">
         <v>547</v>
       </c>
-      <c r="E140" s="7">
-        <v>1</v>
-      </c>
-      <c r="F140" s="8">
+      <c r="E140" s="6">
+        <v>1</v>
+      </c>
+      <c r="F140" s="7">
         <f>VLOOKUP(D140,'Final Data'!$G:$J,3,FALSE)</f>
         <v>126667</v>
       </c>
-      <c r="G140" s="8">
+      <c r="G140" s="7">
         <f>VLOOKUP(D140,'Final Data'!$G:$J,4,FALSE)</f>
         <v>1714</v>
       </c>
@@ -13563,21 +13570,21 @@
       <c r="A141" t="s">
         <v>592</v>
       </c>
-      <c r="B141" s="7">
+      <c r="B141" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A141)</f>
         <v>1</v>
       </c>
       <c r="D141" t="s">
         <v>565</v>
       </c>
-      <c r="E141" s="7">
-        <v>1</v>
-      </c>
-      <c r="F141" s="11">
+      <c r="E141" s="6">
+        <v>1</v>
+      </c>
+      <c r="F141" s="10">
         <f>VLOOKUP(D141,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G141" s="11">
+      <c r="G141" s="10">
         <f>VLOOKUP(D141,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13586,21 +13593,21 @@
       <c r="A142" t="s">
         <v>593</v>
       </c>
-      <c r="B142" s="7">
+      <c r="B142" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A142)</f>
         <v>1</v>
       </c>
       <c r="D142" t="s">
         <v>566</v>
       </c>
-      <c r="E142" s="7">
-        <v>1</v>
-      </c>
-      <c r="F142" s="8">
+      <c r="E142" s="6">
+        <v>1</v>
+      </c>
+      <c r="F142" s="7">
         <f>VLOOKUP(D142,'Final Data'!$G:$J,3,FALSE)</f>
         <v>122321</v>
       </c>
-      <c r="G142" s="8">
+      <c r="G142" s="7">
         <f>VLOOKUP(D142,'Final Data'!$G:$J,4,FALSE)</f>
         <v>4051</v>
       </c>
@@ -13609,21 +13616,21 @@
       <c r="A143" t="s">
         <v>597</v>
       </c>
-      <c r="B143" s="7">
+      <c r="B143" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A143)</f>
         <v>1</v>
       </c>
       <c r="D143" t="s">
         <v>574</v>
       </c>
-      <c r="E143" s="7">
-        <v>1</v>
-      </c>
-      <c r="F143" s="8">
+      <c r="E143" s="6">
+        <v>1</v>
+      </c>
+      <c r="F143" s="7">
         <f>VLOOKUP(D143,'Final Data'!$G:$J,3,FALSE)</f>
         <v>52397</v>
       </c>
-      <c r="G143" s="8">
+      <c r="G143" s="7">
         <f>VLOOKUP(D143,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10644</v>
       </c>
@@ -13632,21 +13639,21 @@
       <c r="A144" t="s">
         <v>600</v>
       </c>
-      <c r="B144" s="7">
+      <c r="B144" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A144)</f>
         <v>1</v>
       </c>
       <c r="D144" t="s">
         <v>577</v>
       </c>
-      <c r="E144" s="7">
-        <v>1</v>
-      </c>
-      <c r="F144" s="11">
+      <c r="E144" s="6">
+        <v>1</v>
+      </c>
+      <c r="F144" s="10">
         <f>VLOOKUP(D144,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G144" s="11">
+      <c r="G144" s="10">
         <f>VLOOKUP(D144,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13655,21 +13662,21 @@
       <c r="A145" t="s">
         <v>601</v>
       </c>
-      <c r="B145" s="7">
+      <c r="B145" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A145)</f>
         <v>1</v>
       </c>
       <c r="D145" t="s">
         <v>583</v>
       </c>
-      <c r="E145" s="7">
-        <v>1</v>
-      </c>
-      <c r="F145" s="8">
+      <c r="E145" s="6">
+        <v>1</v>
+      </c>
+      <c r="F145" s="7">
         <f>VLOOKUP(D145,'Final Data'!$G:$J,3,FALSE)</f>
         <v>72731</v>
       </c>
-      <c r="G145" s="8">
+      <c r="G145" s="7">
         <f>VLOOKUP(D145,'Final Data'!$G:$J,4,FALSE)</f>
         <v>12234</v>
       </c>
@@ -13678,21 +13685,21 @@
       <c r="A146" t="s">
         <v>605</v>
       </c>
-      <c r="B146" s="7">
+      <c r="B146" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A146)</f>
         <v>1</v>
       </c>
       <c r="D146" t="s">
         <v>592</v>
       </c>
-      <c r="E146" s="7">
-        <v>1</v>
-      </c>
-      <c r="F146" s="8">
+      <c r="E146" s="6">
+        <v>1</v>
+      </c>
+      <c r="F146" s="7">
         <f>VLOOKUP(D146,'Final Data'!$G:$J,3,FALSE)</f>
         <v>113815</v>
       </c>
-      <c r="G146" s="8">
+      <c r="G146" s="7">
         <f>VLOOKUP(D146,'Final Data'!$G:$J,4,FALSE)</f>
         <v>45602</v>
       </c>
@@ -13701,21 +13708,21 @@
       <c r="A147" t="s">
         <v>608</v>
       </c>
-      <c r="B147" s="7">
+      <c r="B147" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A147)</f>
         <v>3</v>
       </c>
       <c r="D147" t="s">
         <v>593</v>
       </c>
-      <c r="E147" s="7">
-        <v>1</v>
-      </c>
-      <c r="F147" s="11">
+      <c r="E147" s="6">
+        <v>1</v>
+      </c>
+      <c r="F147" s="10">
         <f>VLOOKUP(D147,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G147" s="11">
+      <c r="G147" s="10">
         <f>VLOOKUP(D147,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -13724,21 +13731,21 @@
       <c r="A148" t="s">
         <v>615</v>
       </c>
-      <c r="B148" s="7">
+      <c r="B148" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A148)</f>
         <v>1</v>
       </c>
       <c r="D148" t="s">
         <v>597</v>
       </c>
-      <c r="E148" s="7">
-        <v>1</v>
-      </c>
-      <c r="F148" s="8">
+      <c r="E148" s="6">
+        <v>1</v>
+      </c>
+      <c r="F148" s="7">
         <f>VLOOKUP(D148,'Final Data'!$G:$J,3,FALSE)</f>
         <v>91889</v>
       </c>
-      <c r="G148" s="8">
+      <c r="G148" s="7">
         <f>VLOOKUP(D148,'Final Data'!$G:$J,4,FALSE)</f>
         <v>24154</v>
       </c>
@@ -13747,21 +13754,21 @@
       <c r="A149" t="s">
         <v>618</v>
       </c>
-      <c r="B149" s="7">
+      <c r="B149" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A149)</f>
         <v>2</v>
       </c>
       <c r="D149" t="s">
         <v>600</v>
       </c>
-      <c r="E149" s="7">
-        <v>1</v>
-      </c>
-      <c r="F149" s="8">
+      <c r="E149" s="6">
+        <v>1</v>
+      </c>
+      <c r="F149" s="7">
         <f>VLOOKUP(D149,'Final Data'!$G:$J,3,FALSE)</f>
         <v>88679</v>
       </c>
-      <c r="G149" s="8">
+      <c r="G149" s="7">
         <f>VLOOKUP(D149,'Final Data'!$G:$J,4,FALSE)</f>
         <v>2980</v>
       </c>
@@ -13770,21 +13777,21 @@
       <c r="A150" t="s">
         <v>623</v>
       </c>
-      <c r="B150" s="7">
+      <c r="B150" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A150)</f>
         <v>3</v>
       </c>
       <c r="D150" t="s">
         <v>601</v>
       </c>
-      <c r="E150" s="7">
-        <v>1</v>
-      </c>
-      <c r="F150" s="8">
+      <c r="E150" s="6">
+        <v>1</v>
+      </c>
+      <c r="F150" s="7">
         <f>VLOOKUP(D150,'Final Data'!$G:$J,3,FALSE)</f>
         <v>132443</v>
       </c>
-      <c r="G150" s="8">
+      <c r="G150" s="7">
         <f>VLOOKUP(D150,'Final Data'!$G:$J,4,FALSE)</f>
         <v>22155</v>
       </c>
@@ -13793,21 +13800,21 @@
       <c r="A151" t="s">
         <v>630</v>
       </c>
-      <c r="B151" s="7">
+      <c r="B151" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A151)</f>
         <v>1</v>
       </c>
       <c r="D151" t="s">
         <v>605</v>
       </c>
-      <c r="E151" s="7">
-        <v>1</v>
-      </c>
-      <c r="F151" s="8">
+      <c r="E151" s="6">
+        <v>1</v>
+      </c>
+      <c r="F151" s="7">
         <f>VLOOKUP(D151,'Final Data'!$G:$J,3,FALSE)</f>
         <v>79206</v>
       </c>
-      <c r="G151" s="8">
+      <c r="G151" s="7">
         <f>VLOOKUP(D151,'Final Data'!$G:$J,4,FALSE)</f>
         <v>17902</v>
       </c>
@@ -13816,21 +13823,21 @@
       <c r="A152" t="s">
         <v>635</v>
       </c>
-      <c r="B152" s="7">
+      <c r="B152" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A152)</f>
         <v>1</v>
       </c>
       <c r="D152" t="s">
         <v>615</v>
       </c>
-      <c r="E152" s="7">
-        <v>1</v>
-      </c>
-      <c r="F152" s="8">
+      <c r="E152" s="6">
+        <v>1</v>
+      </c>
+      <c r="F152" s="7">
         <f>VLOOKUP(D152,'Final Data'!$G:$J,3,FALSE)</f>
         <v>35524</v>
       </c>
-      <c r="G152" s="8">
+      <c r="G152" s="7">
         <f>VLOOKUP(D152,'Final Data'!$G:$J,4,FALSE)</f>
         <v>84867</v>
       </c>
@@ -13839,21 +13846,21 @@
       <c r="A153" t="s">
         <v>639</v>
       </c>
-      <c r="B153" s="7">
+      <c r="B153" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A153)</f>
         <v>1</v>
       </c>
       <c r="D153" t="s">
         <v>630</v>
       </c>
-      <c r="E153" s="7">
-        <v>1</v>
-      </c>
-      <c r="F153" s="8">
+      <c r="E153" s="6">
+        <v>1</v>
+      </c>
+      <c r="F153" s="7">
         <f>VLOOKUP(D153,'Final Data'!$G:$J,3,FALSE)</f>
         <v>90805</v>
       </c>
-      <c r="G153" s="8">
+      <c r="G153" s="7">
         <f>VLOOKUP(D153,'Final Data'!$G:$J,4,FALSE)</f>
         <v>22572</v>
       </c>
@@ -13862,21 +13869,21 @@
       <c r="A154" t="s">
         <v>640</v>
       </c>
-      <c r="B154" s="7">
+      <c r="B154" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A154)</f>
         <v>1</v>
       </c>
       <c r="D154" t="s">
         <v>635</v>
       </c>
-      <c r="E154" s="7">
-        <v>1</v>
-      </c>
-      <c r="F154" s="8">
+      <c r="E154" s="6">
+        <v>1</v>
+      </c>
+      <c r="F154" s="7">
         <f>VLOOKUP(D154,'Final Data'!$G:$J,3,FALSE)</f>
         <v>51113</v>
       </c>
-      <c r="G154" s="8">
+      <c r="G154" s="7">
         <f>VLOOKUP(D154,'Final Data'!$G:$J,4,FALSE)</f>
         <v>60824</v>
       </c>
@@ -13885,21 +13892,21 @@
       <c r="A155" t="s">
         <v>644</v>
       </c>
-      <c r="B155" s="7">
+      <c r="B155" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A155)</f>
         <v>1</v>
       </c>
       <c r="D155" t="s">
         <v>639</v>
       </c>
-      <c r="E155" s="7">
-        <v>1</v>
-      </c>
-      <c r="F155" s="8">
+      <c r="E155" s="6">
+        <v>1</v>
+      </c>
+      <c r="F155" s="7">
         <f>VLOOKUP(D155,'Final Data'!$G:$J,3,FALSE)</f>
         <v>85199</v>
       </c>
-      <c r="G155" s="8">
+      <c r="G155" s="7">
         <f>VLOOKUP(D155,'Final Data'!$G:$J,4,FALSE)</f>
         <v>29386</v>
       </c>
@@ -13908,21 +13915,21 @@
       <c r="A156" t="s">
         <v>647</v>
       </c>
-      <c r="B156" s="7">
+      <c r="B156" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A156)</f>
         <v>6</v>
       </c>
       <c r="D156" t="s">
         <v>640</v>
       </c>
-      <c r="E156" s="7">
-        <v>1</v>
-      </c>
-      <c r="F156" s="8">
+      <c r="E156" s="6">
+        <v>1</v>
+      </c>
+      <c r="F156" s="7">
         <f>VLOOKUP(D156,'Final Data'!$G:$J,3,FALSE)</f>
         <v>154647</v>
       </c>
-      <c r="G156" s="8">
+      <c r="G156" s="7">
         <f>VLOOKUP(D156,'Final Data'!$G:$J,4,FALSE)</f>
         <v>15998</v>
       </c>
@@ -13931,21 +13938,21 @@
       <c r="A157" t="s">
         <v>659</v>
       </c>
-      <c r="B157" s="7">
+      <c r="B157" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A157)</f>
         <v>1</v>
       </c>
       <c r="D157" t="s">
         <v>644</v>
       </c>
-      <c r="E157" s="7">
-        <v>1</v>
-      </c>
-      <c r="F157" s="8">
+      <c r="E157" s="6">
+        <v>1</v>
+      </c>
+      <c r="F157" s="7">
         <f>VLOOKUP(D157,'Final Data'!$G:$J,3,FALSE)</f>
         <v>121678</v>
       </c>
-      <c r="G157" s="8">
+      <c r="G157" s="7">
         <f>VLOOKUP(D157,'Final Data'!$G:$J,4,FALSE)</f>
         <v>5961</v>
       </c>
@@ -13954,21 +13961,21 @@
       <c r="A158" t="s">
         <v>661</v>
       </c>
-      <c r="B158" s="7">
+      <c r="B158" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A158)</f>
         <v>1</v>
       </c>
       <c r="D158" t="s">
         <v>659</v>
       </c>
-      <c r="E158" s="7">
-        <v>1</v>
-      </c>
-      <c r="F158" s="8">
+      <c r="E158" s="6">
+        <v>1</v>
+      </c>
+      <c r="F158" s="7">
         <f>VLOOKUP(D158,'Final Data'!$G:$J,3,FALSE)</f>
         <v>105931</v>
       </c>
-      <c r="G158" s="8">
+      <c r="G158" s="7">
         <f>VLOOKUP(D158,'Final Data'!$G:$J,4,FALSE)</f>
         <v>10932</v>
       </c>
@@ -13977,21 +13984,21 @@
       <c r="A159" t="s">
         <v>663</v>
       </c>
-      <c r="B159" s="7">
+      <c r="B159" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A159)</f>
         <v>1</v>
       </c>
       <c r="D159" t="s">
         <v>661</v>
       </c>
-      <c r="E159" s="7">
-        <v>1</v>
-      </c>
-      <c r="F159" s="8">
+      <c r="E159" s="6">
+        <v>1</v>
+      </c>
+      <c r="F159" s="7">
         <f>VLOOKUP(D159,'Final Data'!$G:$J,3,FALSE)</f>
         <v>50477</v>
       </c>
-      <c r="G159" s="8">
+      <c r="G159" s="7">
         <f>VLOOKUP(D159,'Final Data'!$G:$J,4,FALSE)</f>
         <v>53345</v>
       </c>
@@ -14000,21 +14007,21 @@
       <c r="A160" t="s">
         <v>668</v>
       </c>
-      <c r="B160" s="7">
+      <c r="B160" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A160)</f>
         <v>1</v>
       </c>
       <c r="D160" t="s">
         <v>663</v>
       </c>
-      <c r="E160" s="7">
-        <v>1</v>
-      </c>
-      <c r="F160" s="8">
+      <c r="E160" s="6">
+        <v>1</v>
+      </c>
+      <c r="F160" s="7">
         <f>VLOOKUP(D160,'Final Data'!$G:$J,3,FALSE)</f>
         <v>159923</v>
       </c>
-      <c r="G160" s="8">
+      <c r="G160" s="7">
         <f>VLOOKUP(D160,'Final Data'!$G:$J,4,FALSE)</f>
         <v>30591</v>
       </c>
@@ -14023,21 +14030,21 @@
       <c r="A161" t="s">
         <v>672</v>
       </c>
-      <c r="B161" s="7">
+      <c r="B161" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A161)</f>
         <v>3</v>
       </c>
       <c r="D161" t="s">
         <v>668</v>
       </c>
-      <c r="E161" s="7">
-        <v>1</v>
-      </c>
-      <c r="F161" s="8">
+      <c r="E161" s="6">
+        <v>1</v>
+      </c>
+      <c r="F161" s="7">
         <f>VLOOKUP(D161,'Final Data'!$G:$J,3,FALSE)</f>
         <v>95685</v>
       </c>
-      <c r="G161" s="8">
+      <c r="G161" s="7">
         <f>VLOOKUP(D161,'Final Data'!$G:$J,4,FALSE)</f>
         <v>11246</v>
       </c>
@@ -14046,21 +14053,21 @@
       <c r="A162" t="s">
         <v>679</v>
       </c>
-      <c r="B162" s="7">
+      <c r="B162" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A162)</f>
         <v>1</v>
       </c>
       <c r="D162" t="s">
         <v>679</v>
       </c>
-      <c r="E162" s="7">
-        <v>1</v>
-      </c>
-      <c r="F162" s="8">
+      <c r="E162" s="6">
+        <v>1</v>
+      </c>
+      <c r="F162" s="7">
         <f>VLOOKUP(D162,'Final Data'!$G:$J,3,FALSE)</f>
         <v>161250</v>
       </c>
-      <c r="G162" s="8">
+      <c r="G162" s="7">
         <f>VLOOKUP(D162,'Final Data'!$G:$J,4,FALSE)</f>
         <v>5868</v>
       </c>
@@ -14069,21 +14076,21 @@
       <c r="A163" t="s">
         <v>680</v>
       </c>
-      <c r="B163" s="7">
+      <c r="B163" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A163)</f>
         <v>1</v>
       </c>
       <c r="D163" t="s">
         <v>680</v>
       </c>
-      <c r="E163" s="7">
-        <v>1</v>
-      </c>
-      <c r="F163" s="8">
+      <c r="E163" s="6">
+        <v>1</v>
+      </c>
+      <c r="F163" s="7">
         <f>VLOOKUP(D163,'Final Data'!$G:$J,3,FALSE)</f>
         <v>147463</v>
       </c>
-      <c r="G163" s="8">
+      <c r="G163" s="7">
         <f>VLOOKUP(D163,'Final Data'!$G:$J,4,FALSE)</f>
         <v>17231</v>
       </c>
@@ -14092,21 +14099,21 @@
       <c r="A164" t="s">
         <v>684</v>
       </c>
-      <c r="B164" s="7">
+      <c r="B164" s="6">
         <f>COUNTIF('Final Data'!$G:$G,Analysis!A164)</f>
         <v>1</v>
       </c>
       <c r="D164" t="s">
         <v>684</v>
       </c>
-      <c r="E164" s="7">
-        <v>1</v>
-      </c>
-      <c r="F164" s="11">
+      <c r="E164" s="6">
+        <v>1</v>
+      </c>
+      <c r="F164" s="10">
         <f>VLOOKUP(D164,'Final Data'!$G:$J,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G164" s="11">
+      <c r="G164" s="10">
         <f>VLOOKUP(D164,'Final Data'!$G:$J,4,FALSE)</f>
         <v>0</v>
       </c>
@@ -14125,10 +14132,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -14173,7 +14180,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <f>B4/B2</f>
         <v>0.32793522267206476</v>
       </c>
@@ -14182,7 +14189,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <f>20/B1</f>
         <v>0.12345679012345678</v>
       </c>

</xml_diff>